<commit_message>
KCOR should work now for japan data
</commit_message>
<xml_diff>
--- a/data/japan2/KCOR_summary.xlsx
+++ b/data/japan2/KCOR_summary.xlsx
@@ -6001,7 +6001,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6052,7 +6052,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -6154,7 +6154,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -6205,7 +6205,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -6256,7 +6256,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -6307,7 +6307,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -6358,7 +6358,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -6409,7 +6409,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -6460,7 +6460,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -6511,7 +6511,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -6562,7 +6562,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -6613,7 +6613,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -6664,7 +6664,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -6715,7 +6715,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -6766,7 +6766,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -6817,7 +6817,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -6868,7 +6868,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6919,7 +6919,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6970,7 +6970,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -7021,7 +7021,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -7072,7 +7072,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7123,7 +7123,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -7174,7 +7174,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -7225,7 +7225,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -7276,7 +7276,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -7327,7 +7327,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -7378,7 +7378,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -7429,7 +7429,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -7480,7 +7480,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -7531,7 +7531,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7633,7 +7633,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7684,7 +7684,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7735,7 +7735,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7786,7 +7786,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7837,7 +7837,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7939,7 +7939,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7990,7 +7990,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -8041,7 +8041,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8092,7 +8092,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8143,7 +8143,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8245,7 +8245,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -8296,7 +8296,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8347,7 +8347,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -8398,7 +8398,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8449,7 +8449,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8500,7 +8500,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8551,7 +8551,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -8602,7 +8602,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -8653,7 +8653,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -8704,7 +8704,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -8755,7 +8755,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -8806,7 +8806,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -8857,7 +8857,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -8908,7 +8908,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -8959,7 +8959,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -9010,7 +9010,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-02-27</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -9061,7 +9061,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -9112,7 +9112,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -9163,7 +9163,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -9214,7 +9214,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -9265,7 +9265,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -9316,7 +9316,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -9367,7 +9367,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -9418,7 +9418,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -9469,7 +9469,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -9520,7 +9520,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -9571,7 +9571,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -9622,7 +9622,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -9673,7 +9673,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -9724,7 +9724,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -9775,7 +9775,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -9826,7 +9826,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -9877,7 +9877,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -9928,7 +9928,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -9979,7 +9979,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -10030,7 +10030,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -10081,7 +10081,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -10132,7 +10132,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -10183,7 +10183,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -10285,7 +10285,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -10336,7 +10336,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -10387,7 +10387,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -10438,7 +10438,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -10489,7 +10489,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -10540,7 +10540,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -10591,7 +10591,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -10642,7 +10642,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -10693,7 +10693,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -10744,7 +10744,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -10795,7 +10795,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -10846,7 +10846,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -10897,7 +10897,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -10948,7 +10948,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -10999,7 +10999,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -11050,7 +11050,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -11101,7 +11101,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -11152,7 +11152,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -11203,7 +11203,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -11254,7 +11254,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -11305,7 +11305,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -11356,7 +11356,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -11407,7 +11407,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -11458,7 +11458,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -11509,7 +11509,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -11560,7 +11560,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -11611,7 +11611,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -11662,7 +11662,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -11713,7 +11713,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -11764,7 +11764,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -11815,7 +11815,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -11866,7 +11866,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -11917,7 +11917,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -11968,7 +11968,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -12019,7 +12019,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -12070,7 +12070,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -12121,7 +12121,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -12172,7 +12172,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -12223,7 +12223,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -12274,7 +12274,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -12325,7 +12325,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -12376,7 +12376,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -12427,7 +12427,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -12478,7 +12478,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -12529,7 +12529,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -12580,7 +12580,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -12631,7 +12631,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -12682,7 +12682,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -12733,7 +12733,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -12784,7 +12784,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -12835,7 +12835,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -12886,7 +12886,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -12937,7 +12937,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -12988,7 +12988,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -13039,7 +13039,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -13090,7 +13090,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -13141,7 +13141,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -13192,7 +13192,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -13243,7 +13243,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -13294,7 +13294,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -13345,7 +13345,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -13396,7 +13396,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -13447,7 +13447,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -13498,7 +13498,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -13600,7 +13600,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -13651,7 +13651,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -13702,7 +13702,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -13753,7 +13753,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -13804,7 +13804,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -13855,7 +13855,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -13906,7 +13906,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -13957,7 +13957,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -14059,7 +14059,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -14110,7 +14110,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -14161,7 +14161,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -14212,7 +14212,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -14263,7 +14263,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -14314,7 +14314,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -14365,7 +14365,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -14416,7 +14416,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -14467,7 +14467,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -14518,7 +14518,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -14569,7 +14569,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -14620,7 +14620,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -14671,7 +14671,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -14722,7 +14722,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -14773,7 +14773,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -14824,7 +14824,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -14875,7 +14875,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -14926,7 +14926,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -14977,7 +14977,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -15028,7 +15028,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -15130,7 +15130,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -15181,7 +15181,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -15232,7 +15232,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -15283,7 +15283,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -15334,7 +15334,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -15385,7 +15385,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -15436,7 +15436,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -15487,7 +15487,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -15538,7 +15538,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -15589,7 +15589,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -15640,7 +15640,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -15691,7 +15691,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -15742,7 +15742,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -15793,7 +15793,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -15844,7 +15844,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -15895,7 +15895,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -15946,7 +15946,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -15997,7 +15997,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -16048,7 +16048,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -16099,7 +16099,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -16150,7 +16150,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -16201,7 +16201,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -16252,7 +16252,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -16303,7 +16303,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -16354,7 +16354,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -16405,7 +16405,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -16456,7 +16456,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -16507,7 +16507,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -16558,7 +16558,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -16609,7 +16609,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">

</xml_diff>

<commit_message>
KCOR japan analysis spreadsheet
</commit_message>
<xml_diff>
--- a/data/japan2/KCOR_summary.xlsx
+++ b/data/japan2/KCOR_summary.xlsx
@@ -3577,7 +3577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3874,7 +3874,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3 vs 2</t>
+          <t>3 vs 0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -3891,17 +3891,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.9794</t>
+          <t>0.9963</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.920</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.050</t>
         </is>
       </c>
     </row>
@@ -3914,17 +3914,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0185</t>
+          <t>1.1633</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.300</t>
         </is>
       </c>
     </row>
@@ -3937,17 +3937,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8498</t>
+          <t>1.0099</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.767</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>1.111</t>
         </is>
       </c>
     </row>
@@ -3960,17 +3960,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0453</t>
+          <t>0.9150</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>0.820</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -3983,17 +3983,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8185</t>
+          <t>0.5119</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.671</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>0.611</t>
         </is>
       </c>
     </row>
@@ -4006,17 +4006,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1340</t>
+          <t>0.8995</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.739</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.094</t>
         </is>
       </c>
     </row>
@@ -4029,17 +4029,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2579</t>
+          <t>1.2576</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.911</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.801</t>
+          <t>1.736</t>
         </is>
       </c>
     </row>
@@ -4052,17 +4052,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2.5373</t>
+          <t>2.2856</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.454</t>
+          <t>1.313</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4.427</t>
+          <t>3.979</t>
         </is>
       </c>
     </row>
@@ -4075,17 +4075,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.6409</t>
+          <t>1.5999</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.280</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.469</t>
+          <t>3.347</t>
         </is>
       </c>
     </row>
@@ -4098,17 +4098,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.7500</t>
+          <t>1.4578</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.203</t>
+          <t>0.412</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.765</t>
+          <t>5.159</t>
         </is>
       </c>
     </row>
@@ -4122,7 +4122,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4 vs 0</t>
+          <t>3 vs 2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -4139,17 +4139,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0771</t>
+          <t>0.9794</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.920</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
@@ -4162,17 +4162,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3011</t>
+          <t>1.0185</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>0.878</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>1.181</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -4185,17 +4185,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0658</t>
+          <t>0.8498</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>0.941</t>
         </is>
       </c>
     </row>
@@ -4208,17 +4208,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9306</t>
+          <t>1.0453</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.214</t>
         </is>
       </c>
     </row>
@@ -4231,17 +4231,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.6314</t>
+          <t>0.8185</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.544</t>
+          <t>0.671</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.733</t>
+          <t>0.998</t>
         </is>
       </c>
     </row>
@@ -4254,17 +4254,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.2237</t>
+          <t>1.1340</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.892</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.520</t>
+          <t>1.441</t>
         </is>
       </c>
     </row>
@@ -4277,17 +4277,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.7618</t>
+          <t>1.2579</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.530</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.801</t>
         </is>
       </c>
     </row>
@@ -4300,17 +4300,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2.4288</t>
+          <t>2.5373</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.454</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4.580</t>
+          <t>4.427</t>
         </is>
       </c>
     </row>
@@ -4323,17 +4323,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.1694</t>
+          <t>0.6409</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.280</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.070</t>
+          <t>1.469</t>
         </is>
       </c>
     </row>
@@ -4346,17 +4346,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>4.8673</t>
+          <t>0.7500</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.730</t>
+          <t>0.203</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>13.697</t>
+          <t>2.765</t>
         </is>
       </c>
     </row>
@@ -4370,7 +4370,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4 vs 3</t>
+          <t>4 vs 0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -4387,17 +4387,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.0812</t>
+          <t>1.0771</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.040</t>
+          <t>1.028</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.129</t>
         </is>
       </c>
     </row>
@@ -4410,17 +4410,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.1185</t>
+          <t>1.3011</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -4433,17 +4433,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.0554</t>
+          <t>1.0658</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.979</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.161</t>
         </is>
       </c>
     </row>
@@ -4456,17 +4456,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0171</t>
+          <t>0.9306</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.027</t>
         </is>
       </c>
     </row>
@@ -4479,17 +4479,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.2334</t>
+          <t>0.6314</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>0.544</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>0.733</t>
         </is>
       </c>
     </row>
@@ -4502,17 +4502,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.3604</t>
+          <t>1.2237</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.670</t>
+          <t>1.520</t>
         </is>
       </c>
     </row>
@@ -4525,17 +4525,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.6058</t>
+          <t>0.7618</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.421</t>
+          <t>0.530</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -4548,17 +4548,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0627</t>
+          <t>2.4288</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.571</t>
+          <t>1.288</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.977</t>
+          <t>4.580</t>
         </is>
       </c>
     </row>
@@ -4571,17 +4571,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2.2303</t>
+          <t>1.1694</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.661</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.837</t>
+          <t>2.070</t>
         </is>
       </c>
     </row>
@@ -4594,17 +4594,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>3.3388</t>
+          <t>4.8673</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>1.730</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>11.943</t>
+          <t>13.697</t>
         </is>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5 vs 0</t>
+          <t>4 vs 3</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -4635,17 +4635,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.4030</t>
+          <t>1.0812</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.040</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -4658,17 +4658,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.6451</t>
+          <t>1.1185</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>1.038</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.817</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -4681,17 +4681,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.4251</t>
+          <t>1.0554</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.307</t>
+          <t>0.987</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.553</t>
+          <t>1.128</t>
         </is>
       </c>
     </row>
@@ -4704,17 +4704,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.4006</t>
+          <t>1.0171</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.267</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>1.108</t>
         </is>
       </c>
     </row>
@@ -4727,17 +4727,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.7003</t>
+          <t>1.2334</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.594</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.826</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -4750,17 +4750,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.9054</t>
+          <t>1.3604</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.650</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.670</t>
         </is>
       </c>
     </row>
@@ -4773,17 +4773,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.8159</t>
+          <t>0.6058</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.081</t>
+          <t>0.421</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3.049</t>
+          <t>0.871</t>
         </is>
       </c>
     </row>
@@ -4796,17 +4796,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.4286</t>
+          <t>1.0627</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.075</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2.452</t>
+          <t>1.977</t>
         </is>
       </c>
     </row>
@@ -4819,17 +4819,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2.7520</t>
+          <t>2.2303</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>1.028</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>9.046</t>
+          <t>4.837</t>
         </is>
       </c>
     </row>
@@ -4842,17 +4842,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>3.3388</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>11.943</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5 vs 4</t>
+          <t>5 vs 0</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -4883,17 +4883,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.3025</t>
+          <t>1.4030</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.337</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.473</t>
         </is>
       </c>
     </row>
@@ -4906,17 +4906,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.2644</t>
+          <t>1.6451</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.490</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.817</t>
         </is>
       </c>
     </row>
@@ -4929,17 +4929,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.3371</t>
+          <t>1.4251</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.307</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.409</t>
+          <t>1.553</t>
         </is>
       </c>
     </row>
@@ -4952,17 +4952,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.5050</t>
+          <t>1.4006</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.267</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.619</t>
+          <t>1.549</t>
         </is>
       </c>
     </row>
@@ -4975,17 +4975,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.1092</t>
+          <t>0.7003</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.594</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>0.826</t>
         </is>
       </c>
     </row>
@@ -4998,17 +4998,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.7399</t>
+          <t>0.9054</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.528</t>
+          <t>0.650</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.261</t>
         </is>
       </c>
     </row>
@@ -5021,17 +5021,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2.3836</t>
+          <t>1.8159</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.383</t>
+          <t>1.081</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4.108</t>
+          <t>3.049</t>
         </is>
       </c>
     </row>
@@ -5044,17 +5044,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.1764</t>
+          <t>0.4286</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.030</t>
+          <t>0.075</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>2.452</t>
         </is>
       </c>
     </row>
@@ -5067,17 +5067,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2.3533</t>
+          <t>2.7520</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.700</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>7.911</t>
+          <t>9.046</t>
         </is>
       </c>
     </row>
@@ -5110,6 +5110,254 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>5 vs 4</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>1.3025</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>1.261</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>1.345</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>1.2644</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>1.196</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1.337</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>1.3371</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>1.269</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1.409</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>1.5050</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>1.399</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>1.619</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>1.1092</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>1.277</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.7399</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0.528</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>1.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2.3836</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>1.383</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>4.108</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.1764</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0.030</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>1.032</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2.3533</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0.700</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>7.911</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5122,7 +5370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5419,7 +5667,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3 vs 2</t>
+          <t>3 vs 0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -5436,17 +5684,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.9556</t>
+          <t>0.8593</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.910</t>
         </is>
       </c>
     </row>
@@ -5459,17 +5707,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.7578</t>
+          <t>0.8207</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.644</t>
+          <t>0.724</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.930</t>
         </is>
       </c>
     </row>
@@ -5482,17 +5730,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3360</t>
+          <t>0.9660</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.505</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -5505,17 +5753,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.7218</t>
+          <t>0.8292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.632</t>
+          <t>0.731</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.941</t>
         </is>
       </c>
     </row>
@@ -5528,17 +5776,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8539</t>
+          <t>0.6634</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.694</t>
+          <t>0.567</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.777</t>
         </is>
       </c>
     </row>
@@ -5551,17 +5799,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.2855</t>
+          <t>0.9566</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.225</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.362</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -5574,17 +5822,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0665</t>
+          <t>0.7434</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.751</t>
+          <t>0.568</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.514</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
@@ -5597,17 +5845,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.9349</t>
+          <t>0.8075</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.883</t>
+          <t>1.025</t>
         </is>
       </c>
     </row>
@@ -5620,17 +5868,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.5927</t>
+          <t>0.4572</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.274</t>
+          <t>0.250</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>0.838</t>
         </is>
       </c>
     </row>
@@ -5643,17 +5891,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.9309</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.292</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>2.968</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5915,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4 vs 3</t>
+          <t>3 vs 2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -5684,17 +5932,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0071</t>
+          <t>0.9556</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.063</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -5707,17 +5955,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9302</t>
+          <t>0.7578</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.644</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>0.892</t>
         </is>
       </c>
     </row>
@@ -5730,17 +5978,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.8354</t>
+          <t>1.3360</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.765</t>
+          <t>1.186</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>1.505</t>
         </is>
       </c>
     </row>
@@ -5753,17 +6001,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1153</t>
+          <t>0.7218</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>0.632</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>0.825</t>
         </is>
       </c>
     </row>
@@ -5776,17 +6024,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2116</t>
+          <t>0.8539</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.694</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.427</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -5799,17 +6047,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0213</t>
+          <t>0.2855</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.824</t>
+          <t>0.225</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.266</t>
+          <t>0.362</t>
         </is>
       </c>
     </row>
@@ -5822,17 +6070,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.5773</t>
+          <t>1.0665</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>0.751</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.269</t>
+          <t>1.514</t>
         </is>
       </c>
     </row>
@@ -5845,17 +6093,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.6650</t>
+          <t>1.9349</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.395</t>
+          <t>1.298</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>2.883</t>
         </is>
       </c>
     </row>
@@ -5868,17 +6116,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.0979</t>
+          <t>0.5927</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.427</t>
+          <t>0.274</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.820</t>
+          <t>1.283</t>
         </is>
       </c>
     </row>
@@ -5891,17 +6139,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16.9480</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6.425</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>44.704</t>
+          <t>0.000</t>
         </is>
       </c>
     </row>
@@ -5915,7 +6163,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5 vs 0</t>
+          <t>4 vs 0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -5932,17 +6180,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.8859</t>
+          <t>0.8654</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.927</t>
+          <t>0.911</t>
         </is>
       </c>
     </row>
@@ -5955,17 +6203,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0.8277</t>
+          <t>0.7634</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.753</t>
+          <t>0.686</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.910</t>
+          <t>0.849</t>
         </is>
       </c>
     </row>
@@ -5978,17 +6226,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.7604</t>
+          <t>0.8069</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.703</t>
+          <t>0.739</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.823</t>
+          <t>0.881</t>
         </is>
       </c>
     </row>
@@ -6001,17 +6249,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9927</t>
+          <t>0.9248</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>0.827</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.034</t>
         </is>
       </c>
     </row>
@@ -6024,17 +6272,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.8625</t>
+          <t>0.8038</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.742</t>
+          <t>0.682</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>0.948</t>
         </is>
       </c>
     </row>
@@ -6047,17 +6295,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.8748</t>
+          <t>0.9770</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.798</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.158</t>
+          <t>1.196</t>
         </is>
       </c>
     </row>
@@ -6070,17 +6318,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.2951</t>
+          <t>1.1726</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.175</t>
+          <t>0.854</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.498</t>
+          <t>1.609</t>
         </is>
       </c>
     </row>
@@ -6093,17 +6341,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.3663</t>
+          <t>0.5369</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>0.312</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.644</t>
+          <t>0.925</t>
         </is>
       </c>
     </row>
@@ -6116,17 +6364,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>32.2129</t>
+          <t>0.3050</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>27.287</t>
+          <t>0.143</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>38.028</t>
+          <t>0.651</t>
         </is>
       </c>
     </row>
@@ -6139,17 +6387,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>5.8254</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>2.998</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>11.320</t>
         </is>
       </c>
     </row>
@@ -6163,7 +6411,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5 vs 4</t>
+          <t>4 vs 3</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -6180,17 +6428,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.0237</t>
+          <t>1.0071</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>0.954</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.063</t>
         </is>
       </c>
     </row>
@@ -6203,17 +6451,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0843</t>
+          <t>0.9302</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.168</t>
+          <t>1.039</t>
         </is>
       </c>
     </row>
@@ -6226,17 +6474,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.9424</t>
+          <t>0.8354</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>0.913</t>
         </is>
       </c>
     </row>
@@ -6249,17 +6497,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.0734</t>
+          <t>1.1153</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.178</t>
+          <t>1.261</t>
         </is>
       </c>
     </row>
@@ -6272,17 +6520,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0730</t>
+          <t>1.2116</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>1.029</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.255</t>
+          <t>1.427</t>
         </is>
       </c>
     </row>
@@ -6295,17 +6543,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8954</t>
+          <t>1.0213</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.673</t>
+          <t>0.824</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.266</t>
         </is>
       </c>
     </row>
@@ -6318,17 +6566,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.2517</t>
+          <t>1.5773</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.141</t>
+          <t>1.097</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.448</t>
+          <t>2.269</t>
         </is>
       </c>
     </row>
@@ -6341,17 +6589,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.6821</t>
+          <t>0.6650</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.328</t>
+          <t>0.395</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.416</t>
+          <t>1.120</t>
         </is>
       </c>
     </row>
@@ -6364,17 +6612,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>105.6105</t>
+          <t>1.0979</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>50.274</t>
+          <t>0.427</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>221.857</t>
+          <t>2.820</t>
         </is>
       </c>
     </row>
@@ -6387,17 +6635,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>16.9480</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>6.425</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>44.704</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6659,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6 vs 0</t>
+          <t>5 vs 0</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -6428,17 +6676,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.4620</t>
+          <t>0.8859</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.394</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.533</t>
+          <t>0.927</t>
         </is>
       </c>
     </row>
@@ -6451,17 +6699,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.1702</t>
+          <t>0.8277</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>0.753</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.290</t>
+          <t>0.910</t>
         </is>
       </c>
     </row>
@@ -6474,17 +6722,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.3937</t>
+          <t>0.7604</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.285</t>
+          <t>0.703</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.512</t>
+          <t>0.823</t>
         </is>
       </c>
     </row>
@@ -6497,17 +6745,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.6219</t>
+          <t>0.9927</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.799</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -6520,17 +6768,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2.2357</t>
+          <t>0.8625</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.852</t>
+          <t>0.742</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2.699</t>
+          <t>1.003</t>
         </is>
       </c>
     </row>
@@ -6543,17 +6791,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.7809</t>
+          <t>0.8748</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.519</t>
+          <t>0.661</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.158</t>
         </is>
       </c>
     </row>
@@ -6566,17 +6814,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.6174</t>
+          <t>0.2951</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.370</t>
+          <t>0.175</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>0.498</t>
         </is>
       </c>
     </row>
@@ -6589,17 +6837,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.1792</t>
+          <t>0.3663</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.291</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4.781</t>
+          <t>0.644</t>
         </is>
       </c>
     </row>
@@ -6612,17 +6860,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2.9328</t>
+          <t>32.2129</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.728</t>
+          <t>27.287</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>11.823</t>
+          <t>38.028</t>
         </is>
       </c>
     </row>
@@ -6659,7 +6907,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6 vs 5</t>
+          <t>5 vs 4</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -6676,17 +6924,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.6503</t>
+          <t>1.0237</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.592</t>
+          <t>0.983</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.711</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -6699,17 +6947,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.4138</t>
+          <t>1.0843</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.503</t>
+          <t>1.168</t>
         </is>
       </c>
     </row>
@@ -6722,17 +6970,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1.8329</t>
+          <t>0.9424</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.734</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.938</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -6745,17 +6993,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1.6338</t>
+          <t>1.0734</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>0.978</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1.777</t>
+          <t>1.178</t>
         </is>
       </c>
     </row>
@@ -6768,17 +7016,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2.5922</t>
+          <t>1.0730</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2.161</t>
+          <t>0.917</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3.109</t>
+          <t>1.255</t>
         </is>
       </c>
     </row>
@@ -6791,17 +7039,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>0.8927</t>
+          <t>0.8954</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.567</t>
+          <t>0.673</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.190</t>
         </is>
       </c>
     </row>
@@ -6814,17 +7062,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2.0920</t>
+          <t>0.2517</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>0.141</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>4.223</t>
+          <t>0.448</t>
         </is>
       </c>
     </row>
@@ -6837,17 +7085,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0.5358</t>
+          <t>0.6821</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.122</t>
+          <t>0.328</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2.360</t>
+          <t>1.416</t>
         </is>
       </c>
     </row>
@@ -6860,17 +7108,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.0910</t>
+          <t>105.6105</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.023</t>
+          <t>50.274</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0.364</t>
+          <t>221.857</t>
         </is>
       </c>
     </row>
@@ -6883,17 +7131,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.000</t>
         </is>
       </c>
     </row>
@@ -6903,6 +7151,502 @@
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>6 vs 0</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>1.4620</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>1.394</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>1.533</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>1.1702</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>1.062</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>1.290</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>1.3937</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>1.285</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>1.512</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>1.6219</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>1.463</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>1.799</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2.2357</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>1.852</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2.699</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0.7809</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0.519</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>1.174</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>0.6174</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>0.370</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>1.030</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>1.1792</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0.291</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>4.781</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2.9328</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0.728</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>11.823</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>6 vs 5</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>1.6503</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>1.592</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>1.711</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>1.4138</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>1.330</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>1.503</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>1.8329</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>1.734</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>1.938</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>1.6338</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>1.502</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>1.777</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2.5922</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2.161</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>3.109</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0.8927</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1.406</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2.0920</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>1.036</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>4.223</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0.5358</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0.122</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2.360</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0.0910</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0.364</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>